<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI4-Sandbox@248dc4a73b605dee4c331b65ad129cb2dcbf787e 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-condition-encounter-diagnosis.xlsx
+++ b/StructureDefinition-us-core-condition-encounter-diagnosis.xlsx
@@ -710,7 +710,7 @@
     <t>Valueset to describe the actual problem experienced by the patient</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/condition-code</t>
+    <t>http://hl7.org/fhir/us/core/ValueSet/us-core-condition-code</t>
   </si>
   <si>
     <t>Event.code</t>
@@ -1507,7 +1507,7 @@
     <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="80.05859375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="50.7109375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="54.60546875" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="20.59375" customWidth="true" bestFit="true"/>

</xml_diff>